<commit_message>
Update Feds y Confeds. sector público.xlsx
</commit_message>
<xml_diff>
--- a/Feds y Confeds. sector público.xlsx
+++ b/Feds y Confeds. sector público.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebao\Documents\GitHub\Federaciones-y-Confederaciones-sindicales--1930-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50089C67-BE37-4430-849B-9D4E8345182D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3014AC5-E1ED-447B-ACCB-F440EC960552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leeme" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Año</t>
   </si>
@@ -272,11 +272,11 @@
     </r>
   </si>
   <si>
-    <t>Federaciones sindicales creadas, en receso y vigentes, 1932-2021</t>
+    <t>Federaciones de asociaciones creadas, en receso y vigentes, 1932-2021</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Osorio, Sebastián (2021): "Federaciones sindicales creadas, en receso y vigentes, 1932-2021". En </t>
+      <t xml:space="preserve">Osorio, Sebastián (2021): "Federaciones de asociaciones creadas, en receso y vigentes, 1932-2021". En </t>
     </r>
     <r>
       <rPr>
@@ -303,11 +303,11 @@
     </r>
   </si>
   <si>
-    <t>Confederaciones sindicales creadas, en receso y vigentes, 1932-2021</t>
+    <t>Confederaciones de asociaciones creadas, en receso y vigentes, 1932-2021</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Osorio, Sebastián (2021): "Confederaciones sindicales creadas, en receso y vigentes, 1932-2021". En </t>
+      <t xml:space="preserve">Osorio, Sebastián (2021): "Confederaciones de asociaciones creadas, en receso y vigentes, 1932-2021". En </t>
     </r>
     <r>
       <rPr>
@@ -334,7 +334,35 @@
     </r>
   </si>
   <si>
-    <t>Federaciones y confederaciones sindicales creadas y vigentes, 1932-2021</t>
+    <t>Federaciones y confederaciones de asociaciones creadas y vigentes, 1932-2021</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Osorio, Sebastián (2021): "Federaciones y confederaciones de asociaciones creadas y vigentes, 1932-2021". En </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Repositorio de Estadísticas Sindicales, 1900-2020</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. CIPSTRA, GETSUR y VV.AA. Disponible en: https://repositoriosindical.netlify.app/ </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -426,12 +454,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2510,7 +2538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43AA9F49-4F7B-4F03-81DF-1F0B4E8681F6}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -2604,7 +2632,7 @@
   <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2614,35 +2642,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4451,8 +4479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCC3C7D-90AD-4C20-A21D-B8D06CC2B997}">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4462,35 +4490,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -6295,7 +6323,7 @@
   <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6306,31 +6334,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9" t="s">
-        <v>29</v>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>